<commit_message>
Planning updated after meeting
</commit_message>
<xml_diff>
--- a/planning/Planning.xlsx
+++ b/planning/Planning.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasaelbrecht/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasaelbrecht/Documents/School/Vakken/Semester 2/Computervisie/project/UGent_Computer-Vision-Project/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0D059-67A0-C548-AD7F-4DBD87C928B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DA7D8D-E111-F841-A5E7-0B9AF4C32B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Semi-supervised painting detection (ONLY script)</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>End date</t>
+  </si>
+  <si>
+    <t>Image labelling</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>1 &amp; 2</t>
   </si>
 </sst>
 </file>
@@ -136,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd\ mmmm"/>
+    <numFmt numFmtId="164" formatCode="dd\ mmmm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -246,23 +255,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -320,10 +321,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planning!$A$2:$A$21</c:f>
+              <c:f>Planning!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -383,16 +384,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planning!$B$2:$B$21</c:f>
+              <c:f>Planning!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -409,10 +413,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17</c:v>
@@ -424,33 +428,36 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
@@ -488,10 +495,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planning!$A$2:$A$21</c:f>
+              <c:f>Planning!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -551,16 +558,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planning!$C$2:$C$21</c:f>
+              <c:f>Planning!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -574,19 +584,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -601,13 +611,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>3</c:v>
@@ -616,9 +626,12 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1359,7 +1372,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>334155</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>165497</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1685,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DF0F7A-C142-A64A-96CD-FFAE3B9840B4}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,7 +1780,7 @@
         <v>43924</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E21" si="0">D3+C3</f>
+        <f t="shared" ref="E3:E22" si="0">D3+C3</f>
         <v>43931</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1844,21 +1857,21 @@
         <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9">
         <f>E5</f>
         <v>43932</v>
       </c>
       <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>43934</v>
+        <f>D6+C6</f>
+        <v>43933</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1869,25 +1882,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="9">
-        <f>E6</f>
-        <v>43934</v>
+        <f>E5</f>
+        <v>43932</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>43941</v>
+        <v>43934</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="7">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1895,21 +1910,21 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D8" s="9">
         <f>E7</f>
+        <v>43934</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="E8" s="9">
-        <f>D8+C8</f>
-        <v>43943</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="7">
@@ -1924,18 +1939,18 @@
         <v>17</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="9">
-        <f>D8</f>
+        <f>E8</f>
         <v>43941</v>
       </c>
       <c r="E9" s="9">
         <f>D9+C9</f>
-        <v>43944</v>
+        <v>43943</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="7">
@@ -1950,18 +1965,18 @@
         <v>17</v>
       </c>
       <c r="C10" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="9">
         <f>D9</f>
         <v>43941</v>
       </c>
       <c r="E10" s="9">
-        <f t="shared" si="0"/>
-        <v>43943</v>
+        <f>D10+C10</f>
+        <v>43944</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="7">
@@ -1987,7 +2002,7 @@
         <v>43943</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="7">
@@ -1999,21 +2014,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12" s="9">
-        <f>E9</f>
-        <v>43944</v>
+        <f>D11</f>
+        <v>43941</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>43946</v>
+        <v>43943</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="7">
@@ -2025,25 +2040,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
       </c>
       <c r="D13" s="9">
-        <f>E12</f>
-        <v>43946</v>
+        <f>E10</f>
+        <v>43944</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="0"/>
-        <v>43948</v>
+        <v>43946</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13">
-        <v>3</v>
+      <c r="H13" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2057,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="9">
-        <f>D13</f>
+        <f>E13</f>
         <v>43946</v>
       </c>
       <c r="E14" s="9">
@@ -2065,7 +2080,7 @@
         <v>43948</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14">
@@ -2077,21 +2092,21 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="9">
-        <f>E14</f>
-        <v>43948</v>
+        <f>D14</f>
+        <v>43946</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>43948</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15">
@@ -2109,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="9">
-        <f>D15</f>
+        <f>E15</f>
         <v>43948</v>
       </c>
       <c r="E16" s="9">
@@ -2117,7 +2132,7 @@
         <v>43949</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16">
@@ -2129,25 +2144,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="9">
-        <f>E16</f>
-        <v>43949</v>
+        <f>D16</f>
+        <v>43948</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="0"/>
-        <v>43952</v>
+        <v>43949</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2161,7 +2176,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="9">
-        <f>D17</f>
+        <f>E17</f>
         <v>43949</v>
       </c>
       <c r="E18" s="9">
@@ -2169,7 +2184,7 @@
         <v>43952</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18">
@@ -2181,21 +2196,21 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
       </c>
       <c r="D19" s="9">
-        <f>E18</f>
-        <v>43952</v>
+        <f>D18</f>
+        <v>43949</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="0"/>
-        <v>43955</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>26</v>
+        <v>43952</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19">
@@ -2207,25 +2222,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="9">
         <f>E19</f>
-        <v>43955</v>
+        <v>43952</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="0"/>
-        <v>43959</v>
+        <v>43955</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -2233,24 +2248,50 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" s="9">
         <f>E20</f>
-        <v>43959</v>
+        <v>43955</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="0"/>
+        <v>43959</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9">
+        <f>E21</f>
+        <v>43959</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7">
+      <c r="G22" s="4"/>
+      <c r="H22" s="7">
         <v>5</v>
       </c>
     </row>
@@ -2258,7 +2299,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D14:D18" formula="1"/>
+    <ignoredError sqref="D15:D19 D7" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
First attempt to loosen the timing, dates need to be fixed.
</commit_message>
<xml_diff>
--- a/planning/Planning.xlsx
+++ b/planning/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasaelbrecht/Documents/School/Vakken/Semester 2/Computervisie/project/UGent_Computer-Vision-Project/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ECD628-4597-E948-BECB-D0056F68EF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529827B2-6A8D-E243-A420-B457CDC843BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3140" windowWidth="38400" windowHeight="21140" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
+    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Semi-supervised painting detection (ONLY script)</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Thomas, Gillis, Jochen, Andreas</t>
+  </si>
+  <si>
+    <t>Andreas, Jochen</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -250,6 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,40 +414,40 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -572,10 +576,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
@@ -587,10 +591,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -1677,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DF0F7A-C142-A64A-96CD-FFAE3B9840B4}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,20 +1896,22 @@
         <v>17</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="9">
-        <f>E7</f>
+        <f>D9</f>
         <v>43941</v>
       </c>
       <c r="E8" s="9">
         <f>D8+C8</f>
-        <v>43943</v>
+        <v>43944</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H8" s="7">
         <v>2</v>
       </c>
@@ -1918,21 +1924,21 @@
         <v>17</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9">
-        <f>D8</f>
+        <f>E7</f>
         <v>43941</v>
       </c>
       <c r="E9" s="9">
         <f>D9+C9</f>
-        <v>43944</v>
+        <v>43946</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H9" s="7">
         <v>2</v>
@@ -1943,21 +1949,21 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4">
         <v>2</v>
       </c>
       <c r="D10" s="9">
-        <f>D9</f>
-        <v>43941</v>
+        <f>E9</f>
+        <v>43946</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
-        <v>43943</v>
+        <v>43948</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="7">
@@ -1969,25 +1975,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4">
         <v>2</v>
       </c>
       <c r="D11" s="9">
-        <f>D10</f>
-        <v>43941</v>
+        <f>E10</f>
+        <v>43948</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="0"/>
-        <v>43943</v>
+        <v>43950</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="7">
-        <v>2</v>
+      <c r="H11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1995,25 +2001,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12" s="9">
-        <f>E9</f>
-        <v>43944</v>
+        <f>D11</f>
+        <v>43948</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>43946</v>
+        <v>43950</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="7">
-        <v>2</v>
+      <c r="H12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2021,21 +2027,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="9">
         <f>E12</f>
-        <v>43946</v>
+        <v>43950</v>
       </c>
       <c r="E13" s="9">
-        <f t="shared" si="0"/>
-        <v>43948</v>
+        <f>D13+C13</f>
+        <v>43951</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13">
@@ -2047,21 +2053,21 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="9">
-        <f>D13</f>
-        <v>43946</v>
+        <f>E13</f>
+        <v>43951</v>
       </c>
       <c r="E14" s="9">
-        <f t="shared" si="0"/>
-        <v>43948</v>
+        <f>D14+C14</f>
+        <v>43952</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14">
@@ -2073,18 +2079,18 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="9">
         <f>E14</f>
-        <v>43948</v>
+        <v>43952</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>43953</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>23</v>
@@ -2099,18 +2105,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="9">
         <f>D15</f>
-        <v>43948</v>
+        <v>43952</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>43953</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>24</v>
@@ -2125,18 +2131,18 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="4">
         <v>3</v>
       </c>
       <c r="D17" s="9">
         <f>E16</f>
-        <v>43949</v>
+        <v>43953</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="0"/>
-        <v>43952</v>
+        <v>43956</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>25</v>
@@ -2151,18 +2157,18 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
         <v>3</v>
       </c>
       <c r="D18" s="9">
         <f>D17</f>
-        <v>43949</v>
+        <v>43953</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="0"/>
-        <v>43952</v>
+        <v>43956</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>27</v>
@@ -2177,18 +2183,18 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
       </c>
       <c r="D19" s="9">
         <f>E18</f>
-        <v>43952</v>
+        <v>43956</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="0"/>
-        <v>43955</v>
+        <v>43959</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>26</v>
@@ -2203,18 +2209,18 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4">
         <v>4</v>
       </c>
       <c r="D20" s="9">
         <f>E19</f>
-        <v>43955</v>
+        <v>43959</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="0"/>
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>29</v>
@@ -2229,18 +2235,18 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
       </c>
       <c r="D21" s="9">
         <f>E20</f>
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="0"/>
-        <v>43961</v>
+        <v>43965</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>28</v>
@@ -2249,12 +2255,15 @@
       <c r="H21" s="7">
         <v>5</v>
       </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D24" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D14:D18" formula="1"/>
+    <ignoredError sqref="D16:D18 D12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix wrong dates in Excel
</commit_message>
<xml_diff>
--- a/planning/Planning.xlsx
+++ b/planning/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasaelbrecht/Documents/School/Vakken/Semester 2/Computervisie/project/UGent_Computer-Vision-Project/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529827B2-6A8D-E243-A420-B457CDC843BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D505F-28B0-3842-88DC-382547C5F7F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Semi-supervised painting detection (ONLY script)</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Andreas, Jochen</t>
+  </si>
+  <si>
+    <t>Pieter-Jan, Thomas</t>
   </si>
 </sst>
 </file>
@@ -167,15 +170,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -238,11 +247,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -254,6 +278,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,7 +323,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planning!$B$1</c:f>
+              <c:f>Planning!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +342,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planning!$A$2:$A$21</c:f>
+              <c:f>Planning!$A$4:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -385,7 +411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planning!$B$2:$B$21</c:f>
+              <c:f>Planning!$B$4:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -463,7 +489,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planning!$C$1</c:f>
+              <c:f>Planning!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -484,7 +510,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planning!$A$2:$A$21</c:f>
+              <c:f>Planning!$A$4:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -553,7 +579,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planning!$C$2:$C$21</c:f>
+              <c:f>Planning!$C$4:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1349,13 +1375,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>462549</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>102277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>334155</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>165497</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1681,152 +1707,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DF0F7A-C142-A64A-96CD-FFAE3B9840B4}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="5" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="12">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9">
-        <v>43924</v>
-      </c>
-      <c r="E2" s="9">
-        <f>D2+C2</f>
-        <v>43925</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>7</v>
-      </c>
-      <c r="D3" s="9">
-        <f>D2</f>
-        <v>43924</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E21" si="0">D3+C3</f>
-        <v>43931</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4" s="9">
-        <f>D3</f>
+        <f>$B$1+B4</f>
         <v>43924</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" si="0"/>
-        <v>43931</v>
+        <f>D4+C4</f>
+        <v>43925</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
       <c r="D5" s="9">
-        <f>E4</f>
+        <f t="shared" ref="D5:D23" si="0">$B$1+B5</f>
+        <v>43924</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" ref="E5:E23" si="1">D5+C5</f>
         <v>43931</v>
       </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>43932</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1834,111 +1817,111 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>43924</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="1"/>
+        <v>43931</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
         <v>2</v>
-      </c>
-      <c r="D6" s="9">
-        <f>E5</f>
-        <v>43932</v>
-      </c>
-      <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>43934</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D7" s="9">
-        <f>E6</f>
-        <v>43934</v>
+        <f t="shared" si="0"/>
+        <v>43931</v>
       </c>
       <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>43941</v>
+        <f t="shared" si="1"/>
+        <v>43932</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="7">
         <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="9">
-        <f>D9</f>
-        <v>43941</v>
+        <f t="shared" si="0"/>
+        <v>43932</v>
       </c>
       <c r="E8" s="9">
-        <f>D8+C8</f>
-        <v>43944</v>
+        <f t="shared" si="1"/>
+        <v>43934</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="9">
-        <f>E7</f>
+        <f t="shared" si="0"/>
+        <v>43934</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="1"/>
         <v>43941</v>
       </c>
-      <c r="E9" s="9">
-        <f>D9+C9</f>
-        <v>43946</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="7">
         <v>2</v>
@@ -1946,59 +1929,63 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="9">
-        <f>E9</f>
-        <v>43946</v>
+        <f t="shared" si="0"/>
+        <v>43941</v>
       </c>
       <c r="E10" s="9">
-        <f t="shared" si="0"/>
-        <v>43948</v>
+        <f t="shared" si="1"/>
+        <v>43944</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>43941</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="1"/>
+        <v>43946</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="7">
         <v>2</v>
-      </c>
-      <c r="D11" s="9">
-        <f>E10</f>
-        <v>43948</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="0"/>
-        <v>43950</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>22</v>
@@ -2007,93 +1994,97 @@
         <v>2</v>
       </c>
       <c r="D12" s="9">
-        <f>D11</f>
+        <f t="shared" si="0"/>
+        <v>43946</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="1"/>
         <v>43948</v>
       </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>43950</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12">
-        <v>3</v>
+      <c r="H12" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="9">
-        <f>E12</f>
-        <v>43950</v>
+        <f t="shared" si="0"/>
+        <v>43946</v>
       </c>
       <c r="E13" s="9">
-        <f>D13+C13</f>
-        <v>43951</v>
+        <f t="shared" si="1"/>
+        <v>43948</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="H13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="9">
-        <f>E13</f>
-        <v>43951</v>
+        <f t="shared" si="0"/>
+        <v>43946</v>
       </c>
       <c r="E14" s="9">
-        <f>D14+C14</f>
-        <v>43952</v>
+        <f t="shared" si="1"/>
+        <v>43948</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="H14">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="9">
-        <f>E14</f>
-        <v>43952</v>
+        <f t="shared" si="0"/>
+        <v>43948</v>
       </c>
       <c r="E15" s="9">
-        <f t="shared" si="0"/>
-        <v>43953</v>
+        <f t="shared" si="1"/>
+        <v>43949</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15">
@@ -2102,24 +2093,24 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="9">
-        <f>D15</f>
-        <v>43952</v>
+        <f t="shared" si="0"/>
+        <v>43949</v>
       </c>
       <c r="E16" s="9">
-        <f t="shared" si="0"/>
-        <v>43953</v>
+        <f t="shared" si="1"/>
+        <v>43950</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16">
@@ -2128,76 +2119,76 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="9">
-        <f>E16</f>
-        <v>43953</v>
+        <f t="shared" si="0"/>
+        <v>43950</v>
       </c>
       <c r="E17" s="9">
-        <f t="shared" si="0"/>
-        <v>43956</v>
+        <f t="shared" si="1"/>
+        <v>43951</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="9">
-        <f>D17</f>
-        <v>43953</v>
+        <f t="shared" si="0"/>
+        <v>43950</v>
       </c>
       <c r="E18" s="9">
-        <f t="shared" si="0"/>
-        <v>43956</v>
+        <f t="shared" si="1"/>
+        <v>43951</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
       </c>
       <c r="D19" s="9">
-        <f>E18</f>
-        <v>43956</v>
+        <f t="shared" si="0"/>
+        <v>43951</v>
       </c>
       <c r="E19" s="9">
-        <f t="shared" si="0"/>
-        <v>43959</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>43954</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19">
@@ -2206,65 +2197,114 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="9">
-        <f>E19</f>
-        <v>43959</v>
+        <f t="shared" si="0"/>
+        <v>43951</v>
       </c>
       <c r="E20" s="9">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>43954</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>43954</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" si="1"/>
+        <v>43957</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <v>33</v>
+      </c>
+      <c r="C22" s="4">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>43957</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="1"/>
+        <v>43961</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B23" s="4">
         <v>37</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C23" s="4">
         <v>2</v>
       </c>
-      <c r="D21" s="9">
-        <f>E20</f>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>43961</v>
+      </c>
+      <c r="E23" s="9">
+        <f t="shared" si="1"/>
         <v>43963</v>
       </c>
-      <c r="E21" s="9">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7">
+      <c r="G23" s="4"/>
+      <c r="H23" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D24" s="10"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D26" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D16:D18 D12" formula="1"/>
-  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add name to predict room task
</commit_message>
<xml_diff>
--- a/planning/Planning.xlsx
+++ b/planning/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\UGent_Computer-Vision-Project\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasaelbrecht/Documents/School/Vakken/Semester 2/Computervisie/project/UGent_Computer-Vision-Project/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E377F4D1-44A1-4E5B-A82F-47ADE1BAA609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544672B8-A3A2-464D-8011-9CF9CC4F8C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{AA62CA7A-0168-6A4E-843A-04C73DFE4332}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Semi-supervised painting detection (ONLY script)</t>
   </si>
@@ -134,13 +134,10 @@
     <t>Thomas, Gillis, Jochen, Andreas</t>
   </si>
   <si>
-    <t>Pieter-Jan, Thomas</t>
-  </si>
-  <si>
     <t>Andreas, Jochen, Thomas</t>
   </si>
   <si>
-    <t>Gillis Werrebrouck, Thomas</t>
+    <t>Gillis, Pieter-Jan, Thomas</t>
   </si>
 </sst>
 </file>
@@ -303,7 +300,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -709,7 +706,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1852901520"/>
@@ -768,7 +765,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1852899888"/>
@@ -816,7 +813,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1712,22 +1709,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DF0F7A-C142-A64A-96CD-FFAE3B9840B4}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="150" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.35546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.640625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
@@ -1735,8 +1732,8 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.3" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1762,7 +1759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1790,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1818,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1846,7 +1843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1874,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1902,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1930,7 +1927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1958,7 +1955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1980,13 +1977,13 @@
         <v>15</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2012,7 +2009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2034,13 +2031,13 @@
         <v>21</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2062,13 +2059,13 @@
         <v>20</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2089,12 +2086,14 @@
       <c r="F15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="H15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D26" s="10"/>
     </row>
   </sheetData>

</xml_diff>